<commit_message>
data finished for M_2021_11_Pisek.xlsx
</commit_message>
<xml_diff>
--- a/data/men/M_2021_11_Pisek.xlsx
+++ b/data/men/M_2021_11_Pisek.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jzelenka\Documents\python_j\fencing\data\men\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B348F9F-A429-4198-98DF-3886116816A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07DCEE5-16A9-4EB9-8C47-5040E5EDFBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="-14628" windowWidth="19536" windowHeight="13260" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11280" yWindow="-14580" windowWidth="14880" windowHeight="12360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initiation" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="eliminations" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">eliminations!$A$1:$K$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">first_round!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">initiation!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pools!$A$1:$K$1</definedName>
@@ -63,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4917" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5936" uniqueCount="154">
   <si>
     <t>LUŠTICKÝ Josef</t>
   </si>
@@ -508,13 +509,31 @@
   <si>
     <t>D</t>
   </si>
+  <si>
+    <t>Eliminace_64</t>
+  </si>
+  <si>
+    <t>Eliminace_32</t>
+  </si>
+  <si>
+    <t>Eliminace_16</t>
+  </si>
+  <si>
+    <t>Eliminace_8</t>
+  </si>
+  <si>
+    <t>Eliminace_4</t>
+  </si>
+  <si>
+    <t>Eliminace_2</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -586,7 +605,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -897,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18553FFA-B042-4E5F-9AFC-B6385F9E335A}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:C24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8353,13 +8372,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K470"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" customWidth="1"/>
     <col min="4" max="4" width="18.44140625" customWidth="1"/>
@@ -24796,12 +24815,4473 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D260D1-8EEE-4B84-BE83-A4EA8BEA63C5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.77734375" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="11" width="8.88671875" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="12">
+        <v>15</v>
+      </c>
+      <c r="K2" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J3" s="12">
+        <v>15</v>
+      </c>
+      <c r="K3" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="12">
+        <v>15</v>
+      </c>
+      <c r="K4" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J5" s="13">
+        <v>9</v>
+      </c>
+      <c r="K5" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" s="13">
+        <v>2</v>
+      </c>
+      <c r="K6" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="12">
+        <v>11</v>
+      </c>
+      <c r="K7" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B8" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J8" s="13">
+        <v>6</v>
+      </c>
+      <c r="K8" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" s="13">
+        <v>10</v>
+      </c>
+      <c r="K9" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="12">
+        <v>15</v>
+      </c>
+      <c r="K10" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="12">
+        <v>15</v>
+      </c>
+      <c r="K11" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J12" s="13">
+        <v>10</v>
+      </c>
+      <c r="K12" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J13" s="13">
+        <v>8</v>
+      </c>
+      <c r="K13" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J14" s="13">
+        <v>12</v>
+      </c>
+      <c r="K14" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="12">
+        <v>15</v>
+      </c>
+      <c r="K15" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J16" s="13">
+        <v>10</v>
+      </c>
+      <c r="K16" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="12">
+        <v>15</v>
+      </c>
+      <c r="K17" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="12">
+        <v>15</v>
+      </c>
+      <c r="K18" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J19" s="13">
+        <v>9</v>
+      </c>
+      <c r="K19" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J20" s="13">
+        <v>7</v>
+      </c>
+      <c r="K20" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B21" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J21" s="13">
+        <v>10</v>
+      </c>
+      <c r="K21" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J22" s="12">
+        <v>15</v>
+      </c>
+      <c r="K22" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J23" s="13">
+        <v>11</v>
+      </c>
+      <c r="K23" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B24" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J24" s="13">
+        <v>8</v>
+      </c>
+      <c r="K24" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J25" s="12">
+        <v>15</v>
+      </c>
+      <c r="K25" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="13">
+        <v>11</v>
+      </c>
+      <c r="K26" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J27" s="13">
+        <v>13</v>
+      </c>
+      <c r="K27" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J28" s="12">
+        <v>15</v>
+      </c>
+      <c r="K28" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B29" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J29" s="12">
+        <v>15</v>
+      </c>
+      <c r="K29" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J30" s="12">
+        <v>15</v>
+      </c>
+      <c r="K30" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B31" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J31" s="12">
+        <v>15</v>
+      </c>
+      <c r="K31" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B32" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J32" s="13">
+        <v>8</v>
+      </c>
+      <c r="K32" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B33" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J33" s="13">
+        <v>13</v>
+      </c>
+      <c r="K33" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B34" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" s="12">
+        <v>15</v>
+      </c>
+      <c r="K34" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J35" s="13">
+        <v>9</v>
+      </c>
+      <c r="K35" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J36" s="12">
+        <v>15</v>
+      </c>
+      <c r="K36" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J37" s="12">
+        <v>15</v>
+      </c>
+      <c r="K37" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B38" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J38" s="13">
+        <v>9</v>
+      </c>
+      <c r="K38" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B39" t="s">
+        <v>135</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J39" s="13">
+        <v>9</v>
+      </c>
+      <c r="K39" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J40" s="12">
+        <v>15</v>
+      </c>
+      <c r="K40" s="12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B41" t="s">
+        <v>135</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I41" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J41" s="12">
+        <v>15</v>
+      </c>
+      <c r="K41" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B42" t="s">
+        <v>135</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I42" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J42" s="12">
+        <v>15</v>
+      </c>
+      <c r="K42" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J43" s="13">
+        <v>3</v>
+      </c>
+      <c r="K43" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E44" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J44" s="13">
+        <v>14</v>
+      </c>
+      <c r="K44" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B45" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I45" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J45" s="12">
+        <v>15</v>
+      </c>
+      <c r="K45" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J46" s="13">
+        <v>10</v>
+      </c>
+      <c r="K46" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B47" t="s">
+        <v>135</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J47" s="13">
+        <v>13</v>
+      </c>
+      <c r="K47" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B48" t="s">
+        <v>135</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I48" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J48" s="12">
+        <v>15</v>
+      </c>
+      <c r="K48" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B49" t="s">
+        <v>135</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J49" s="13">
+        <v>13</v>
+      </c>
+      <c r="K49" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B50" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J50" s="13">
+        <v>8</v>
+      </c>
+      <c r="K50" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B51" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I51" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J51" s="12">
+        <v>15</v>
+      </c>
+      <c r="K51" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J52" s="12">
+        <v>15</v>
+      </c>
+      <c r="K52" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B53" t="s">
+        <v>135</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J53" s="13">
+        <v>6</v>
+      </c>
+      <c r="K53" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B54" t="s">
+        <v>135</v>
+      </c>
+      <c r="C54" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H54" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J54" s="13">
+        <v>11</v>
+      </c>
+      <c r="K54" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="H55" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I55" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J55" s="12">
+        <v>15</v>
+      </c>
+      <c r="K55" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B56" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J56" s="13">
+        <v>8</v>
+      </c>
+      <c r="K56" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="13">
+        <v>8</v>
+      </c>
+      <c r="K57" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="J58" s="13">
+        <v>2</v>
+      </c>
+      <c r="K58" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J59" s="12">
+        <v>15</v>
+      </c>
+      <c r="K59" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B60" t="s">
+        <v>135</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H60" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I60" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J60" s="12">
+        <v>15</v>
+      </c>
+      <c r="K60" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B61" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H61" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J61" s="12">
+        <v>15</v>
+      </c>
+      <c r="K61" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B62" t="s">
+        <v>135</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G62" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J62" s="12">
+        <v>15</v>
+      </c>
+      <c r="K62" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B63" t="s">
+        <v>135</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="J63" s="12">
+        <v>15</v>
+      </c>
+      <c r="K63" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B64" t="s">
+        <v>135</v>
+      </c>
+      <c r="C64" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="J64" s="13">
+        <v>15</v>
+      </c>
+      <c r="K64" s="13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B65" t="s">
+        <v>135</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F65" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G65" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H65" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="I65" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J65" s="16">
+        <v>15</v>
+      </c>
+      <c r="K65" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B66" t="s">
+        <v>135</v>
+      </c>
+      <c r="C66" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F66" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G66" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H66" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I66" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J66" s="16">
+        <v>15</v>
+      </c>
+      <c r="K66" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B67" t="s">
+        <v>135</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F67" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G67" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I67" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J67" s="18">
+        <v>11</v>
+      </c>
+      <c r="K67" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B68" t="s">
+        <v>135</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G68" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H68" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I68" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J68" s="18">
+        <v>6</v>
+      </c>
+      <c r="K68" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B69" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G69" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="I69" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J69" s="18">
+        <v>14</v>
+      </c>
+      <c r="K69" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B70" t="s">
+        <v>135</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G70" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H70" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J70" s="16">
+        <v>15</v>
+      </c>
+      <c r="K70" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B71" t="s">
+        <v>135</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F71" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G71" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H71" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I71" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J71" s="18">
+        <v>5</v>
+      </c>
+      <c r="K71" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B72" t="s">
+        <v>135</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I72" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J72" s="16">
+        <v>15</v>
+      </c>
+      <c r="K72" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F73" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H73" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I73" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J73" s="18">
+        <v>8</v>
+      </c>
+      <c r="K73" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F74" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G74" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="H74" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I74" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J74" s="18">
+        <v>9</v>
+      </c>
+      <c r="K74" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G75" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H75" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I75" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J75" s="18">
+        <v>11</v>
+      </c>
+      <c r="K75" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B76" t="s">
+        <v>135</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H76" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I76" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J76" s="16">
+        <v>15</v>
+      </c>
+      <c r="K76" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B77" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F77" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G77" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H77" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I77" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J77" s="16">
+        <v>15</v>
+      </c>
+      <c r="K77" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B78" t="s">
+        <v>135</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G78" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H78" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I78" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J78" s="16">
+        <v>15</v>
+      </c>
+      <c r="K78" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B79" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F79" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G79" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I79" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J79" s="16">
+        <v>15</v>
+      </c>
+      <c r="K79" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B80" t="s">
+        <v>135</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F80" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="G80" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H80" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I80" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J80" s="18">
+        <v>12</v>
+      </c>
+      <c r="K80" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B81" t="s">
+        <v>135</v>
+      </c>
+      <c r="C81" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F81" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H81" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I81" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J81" s="16">
+        <v>15</v>
+      </c>
+      <c r="K81" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B82" t="s">
+        <v>135</v>
+      </c>
+      <c r="C82" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H82" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I82" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J82" s="16">
+        <v>15</v>
+      </c>
+      <c r="K82" s="16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B83" t="s">
+        <v>135</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H83" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I83" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J83" s="16">
+        <v>15</v>
+      </c>
+      <c r="K83" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B84" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F84" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G84" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="H84" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I84" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J84" s="18">
+        <v>9</v>
+      </c>
+      <c r="K84" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B85" t="s">
+        <v>135</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F85" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G85" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I85" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J85" s="18">
+        <v>9</v>
+      </c>
+      <c r="K85" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B86" t="s">
+        <v>135</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F86" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G86" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="H86" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I86" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J86" s="18">
+        <v>10</v>
+      </c>
+      <c r="K86" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B87" t="s">
+        <v>135</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G87" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="H87" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I87" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J87" s="16">
+        <v>15</v>
+      </c>
+      <c r="K87" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B88" t="s">
+        <v>135</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F88" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G88" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I88" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J88" s="18">
+        <v>5</v>
+      </c>
+      <c r="K88" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B89" t="s">
+        <v>135</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G89" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H89" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I89" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J89" s="16">
+        <v>15</v>
+      </c>
+      <c r="K89" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B90" t="s">
+        <v>135</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F90" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G90" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H90" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I90" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J90" s="18">
+        <v>13</v>
+      </c>
+      <c r="K90" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A91" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B91" t="s">
+        <v>135</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F91" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G91" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H91" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J91" s="18">
+        <v>9</v>
+      </c>
+      <c r="K91" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A92" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B92" t="s">
+        <v>135</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F92" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G92" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="H92" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I92" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J92" s="18">
+        <v>8</v>
+      </c>
+      <c r="K92" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B93" t="s">
+        <v>135</v>
+      </c>
+      <c r="C93" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G93" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H93" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I93" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J93" s="16">
+        <v>15</v>
+      </c>
+      <c r="K93" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B94" t="s">
+        <v>135</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G94" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="H94" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I94" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J94" s="16">
+        <v>15</v>
+      </c>
+      <c r="K94" s="16">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B95" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F95" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G95" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I95" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J95" s="18">
+        <v>13</v>
+      </c>
+      <c r="K95" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B96" t="s">
+        <v>135</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E96" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G96" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I96" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J96" s="16">
+        <v>15</v>
+      </c>
+      <c r="K96" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B97" t="s">
+        <v>135</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E97" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F97" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G97" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H97" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I97" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J97" s="16">
+        <v>15</v>
+      </c>
+      <c r="K97" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B98" t="s">
+        <v>135</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E98" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F98" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G98" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H98" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I98" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J98" s="16">
+        <v>15</v>
+      </c>
+      <c r="K98" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B99" t="s">
+        <v>135</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F99" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="G99" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H99" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I99" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J99" s="16">
+        <v>15</v>
+      </c>
+      <c r="K99" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B100" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E100" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F100" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G100" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H100" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I100" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J100" s="16">
+        <v>15</v>
+      </c>
+      <c r="K100" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A101" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B101" t="s">
+        <v>135</v>
+      </c>
+      <c r="C101" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D101" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E101" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F101" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="G101" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H101" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I101" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J101" s="18">
+        <v>14</v>
+      </c>
+      <c r="K101" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B102" t="s">
+        <v>135</v>
+      </c>
+      <c r="C102" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E102" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F102" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G102" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H102" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I102" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J102" s="18">
+        <v>8</v>
+      </c>
+      <c r="K102" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B103" t="s">
+        <v>135</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F103" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G103" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="H103" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I103" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J103" s="16">
+        <v>15</v>
+      </c>
+      <c r="K103" s="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A104" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B104" t="s">
+        <v>135</v>
+      </c>
+      <c r="C104" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D104" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E104" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F104" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G104" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H104" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I104" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J104" s="18">
+        <v>11</v>
+      </c>
+      <c r="K104" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B105" t="s">
+        <v>135</v>
+      </c>
+      <c r="C105" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D105" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F105" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G105" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H105" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I105" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J105" s="18">
+        <v>12</v>
+      </c>
+      <c r="K105" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B106" t="s">
+        <v>135</v>
+      </c>
+      <c r="C106" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D106" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E106" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F106" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G106" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H106" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="I106" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J106" s="16">
+        <v>15</v>
+      </c>
+      <c r="K106" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A107" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B107" t="s">
+        <v>135</v>
+      </c>
+      <c r="C107" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D107" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E107" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F107" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G107" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H107" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I107" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J107" s="18">
+        <v>8</v>
+      </c>
+      <c r="K107" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A108" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B108" t="s">
+        <v>135</v>
+      </c>
+      <c r="C108" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D108" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F108" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G108" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="H108" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I108" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J108" s="18">
+        <v>14</v>
+      </c>
+      <c r="K108" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A109" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B109" t="s">
+        <v>135</v>
+      </c>
+      <c r="C109" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D109" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E109" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F109" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G109" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H109" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I109" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J109" s="18">
+        <v>8</v>
+      </c>
+      <c r="K109" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B110" t="s">
+        <v>135</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E110" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G110" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H110" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I110" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J110" s="16">
+        <v>15</v>
+      </c>
+      <c r="K110" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B111" t="s">
+        <v>135</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E111" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G111" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="H111" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="I111" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J111" s="16">
+        <v>15</v>
+      </c>
+      <c r="K111" s="16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A112" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B112" t="s">
+        <v>135</v>
+      </c>
+      <c r="C112" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F112" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G112" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H112" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I112" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J112" s="18">
+        <v>6</v>
+      </c>
+      <c r="K112" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B113" t="s">
+        <v>135</v>
+      </c>
+      <c r="C113" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E113" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G113" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H113" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="I113" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J113" s="16">
+        <v>15</v>
+      </c>
+      <c r="K113" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B114" t="s">
+        <v>135</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E114" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G114" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H114" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I114" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J114" s="16">
+        <v>15</v>
+      </c>
+      <c r="K114" s="16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A115" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B115" t="s">
+        <v>135</v>
+      </c>
+      <c r="C115" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D115" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E115" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F115" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="G115" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H115" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I115" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J115" s="18">
+        <v>10</v>
+      </c>
+      <c r="K115" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B116" t="s">
+        <v>135</v>
+      </c>
+      <c r="C116" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D116" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E116" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F116" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G116" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H116" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I116" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J116" s="18">
+        <v>9</v>
+      </c>
+      <c r="K116" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B117" t="s">
+        <v>135</v>
+      </c>
+      <c r="C117" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E117" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G117" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H117" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="I117" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J117" s="16">
+        <v>15</v>
+      </c>
+      <c r="K117" s="16">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A118" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B118" t="s">
+        <v>135</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E118" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F118" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G118" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H118" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I118" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J118" s="18">
+        <v>7</v>
+      </c>
+      <c r="K118" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A119" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B119" t="s">
+        <v>135</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G119" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H119" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I119" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J119" s="18">
+        <v>11</v>
+      </c>
+      <c r="K119" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B120" t="s">
+        <v>135</v>
+      </c>
+      <c r="C120" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E120" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F120" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G120" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H120" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I120" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J120" s="16">
+        <v>15</v>
+      </c>
+      <c r="K120" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B121" t="s">
+        <v>135</v>
+      </c>
+      <c r="C121" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E121" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F121" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="G121" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H121" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I121" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J121" s="18">
+        <v>14</v>
+      </c>
+      <c r="K121" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A122" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D122" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E122" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F122" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G122" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H122" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I122" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J122" s="18">
+        <v>6</v>
+      </c>
+      <c r="K122" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" s="9" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B123" t="s">
+        <v>135</v>
+      </c>
+      <c r="C123" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D123" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E123" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F123" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="G123" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H123" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I123" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J123" s="18">
+        <v>6</v>
+      </c>
+      <c r="K123" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B124" t="s">
+        <v>135</v>
+      </c>
+      <c r="C124" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D124" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E124" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F124" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="G124" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H124" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I124" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J124" s="16">
+        <v>15</v>
+      </c>
+      <c r="K124" s="16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A125" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B125" t="s">
+        <v>135</v>
+      </c>
+      <c r="C125" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D125" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E125" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F125" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="G125" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="H125" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I125" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J125" s="16">
+        <v>15</v>
+      </c>
+      <c r="K125" s="16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B126" t="s">
+        <v>135</v>
+      </c>
+      <c r="C126" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="D126" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E126" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F126" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="G126" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H126" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I126" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J126" s="16">
+        <v>15</v>
+      </c>
+      <c r="K126" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="1">
+        <v>44506</v>
+      </c>
+      <c r="B127" t="s">
+        <v>135</v>
+      </c>
+      <c r="C127" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D127" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E127" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F127" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G127" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="H127" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="I127" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J127" s="18">
+        <v>12</v>
+      </c>
+      <c r="K127" s="18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <autoFilter ref="A1:K127" xr:uid="{E0D260D1-8EEE-4B84-BE83-A4EA8BEA63C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>